<commit_message>
assesment daniel and magnus
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-daniel.xlsx
+++ b/files/assesments/firstround/assesments-daniel.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Self assesment</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Active collaborator, motivated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very active at dicord, Shared a lot of info about machine learning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick response, good at sharing info from lectors </t>
   </si>
 </sst>
 </file>
@@ -556,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -618,8 +624,12 @@
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -704,8 +714,12 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">

</xml_diff>

<commit_message>
Added assessment of Daniel
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-daniel.xlsx
+++ b/files/assesments/firstround/assesments-daniel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanes\OneDrive\Dokumenter\uni\2. semester\epic\files\assesments\firstround\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobvejlinjensen/Honeyjar/files/assesments/firstround/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22280" windowHeight="13240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Self assesment</t>
   </si>
@@ -112,12 +112,18 @@
   </si>
   <si>
     <t>Keeping close contact, and bringing a lot of ideas to the table.</t>
+  </si>
+  <si>
+    <t>Proactive part of the discord server, Motivated to work on the semi-solution for the server problems and machine learning research</t>
+  </si>
+  <si>
+    <t>Good communication over Discord, Good commitments to GitHub and actively sharing files and experiences with other group members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -565,15 +571,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.125" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="3" max="3" width="64.75" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
@@ -599,8 +605,12 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -666,8 +676,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -678,28 +688,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -710,14 +724,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -728,7 +742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -739,50 +753,50 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -823,9 +837,9 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,7 +996,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -991,7 +1005,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1000,7 +1014,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1009,7 +1023,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1018,7 +1032,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1027,7 +1041,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1036,7 +1050,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>